<commit_message>
Extract_invoice_number() return list of invoice_number
</commit_message>
<xml_diff>
--- a/test/get_invoice_id_tests_folder/faktury_id.xlsx
+++ b/test/get_invoice_id_tests_folder/faktury_id.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrowk\Nauka programowania\readingPDF\test\get_invoice_id_tests_folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D8AD4B-E9F8-4CE7-B314-1689BDB97FDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89A704F5-BCB9-444E-A571-C0D9AEAB23EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2475" yWindow="915" windowWidth="15375" windowHeight="7875" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
     <sheet name="One" sheetId="2" r:id="rId2"/>
-    <sheet name="NoSerachColumn" sheetId="6" r:id="rId3"/>
-    <sheet name="Two" sheetId="3" r:id="rId4"/>
+    <sheet name="Two" sheetId="3" r:id="rId3"/>
+    <sheet name="NoSerachColumn" sheetId="6" r:id="rId4"/>
     <sheet name="EmptyTable" sheetId="4" r:id="rId5"/>
     <sheet name="Empty" sheetId="5" r:id="rId6"/>
   </sheets>
@@ -481,7 +481,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,42 +512,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A78E1E09-2C03-4E59-9716-F9C86287EB1C}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92109334-6DC5-4E2C-8FEF-763E54EF3467}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,6 +547,37 @@
       </c>
       <c r="B3" t="s">
         <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A78E1E09-2C03-4E59-9716-F9C86287EB1C}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new_filenames() return list of invoice new filename
</commit_message>
<xml_diff>
--- a/test/get_invoice_id_tests_folder/faktury_id.xlsx
+++ b/test/get_invoice_id_tests_folder/faktury_id.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrowk\Nauka programowania\readingPDF\test\get_invoice_id_tests_folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89A704F5-BCB9-444E-A571-C0D9AEAB23EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F15659-EE24-4F7C-A83C-525E9347D695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2475" yWindow="915" windowWidth="15375" windowHeight="7875" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="15375" windowHeight="7875" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="24">
   <si>
     <t>NR faktury</t>
   </si>
@@ -78,6 +78,30 @@
   </si>
   <si>
     <t>NR faktury1</t>
+  </si>
+  <si>
+    <t>Lp</t>
+  </si>
+  <si>
+    <t>1.</t>
+  </si>
+  <si>
+    <t>4.</t>
+  </si>
+  <si>
+    <t>2.</t>
+  </si>
+  <si>
+    <t>3.</t>
+  </si>
+  <si>
+    <t>5.</t>
+  </si>
+  <si>
+    <t>6.</t>
+  </si>
+  <si>
+    <t>Lp1</t>
   </si>
 </sst>
 </file>
@@ -395,79 +419,100 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B5"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="45.85546875" customWidth="1"/>
+    <col min="2" max="2" width="26" customWidth="1"/>
+    <col min="3" max="3" width="45.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8">
         <v>8492</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>14</v>
       </c>
     </row>
@@ -478,31 +523,37 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83808AB1-7D4A-489B-B777-9AC1D6D71F3F}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -513,39 +564,48 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92109334-6DC5-4E2C-8FEF-763E54EF3467}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
-    <col min="2" max="2" width="44.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="44.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -556,50 +616,62 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A78E1E09-2C03-4E59-9716-F9C86287EB1C}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="30.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80DDE384-D360-4E01-AE4A-06673B0D01E9}">
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80DDE384-D360-4E01-AE4A-06673B0D01E9}">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix test in  move_test
</commit_message>
<xml_diff>
--- a/test/get_invoice_id_tests_folder/faktury_id.xlsx
+++ b/test/get_invoice_id_tests_folder/faktury_id.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7270" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1900" yWindow="1900" windowWidth="14400" windowHeight="7270" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AddComment" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="EmptyTable" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="One" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="NoSerachColumn" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Two" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TheSame" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="EmptyTable" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="One" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="NoSerachColumn" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Two" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -20,7 +21,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="6">
+  <fonts count="9">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -52,6 +53,23 @@
       <sz val="11"/>
     </font>
     <font>
+      <name val="JetBrains Mono"/>
+      <charset val="238"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="238"/>
+      <family val="2"/>
+      <b val="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
       <b val="1"/>
     </font>
   </fonts>
@@ -63,12 +81,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -126,7 +159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -140,7 +173,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -512,29 +554,32 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <cols>
+    <col width="20.1796875" customWidth="1" min="3" max="3"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
+      <c r="A1" s="8" t="inlineStr">
         <is>
           <t>Lp</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="8" t="inlineStr">
         <is>
           <t>NR faktury</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="C1" s="8" t="inlineStr">
         <is>
           <t>nazwa pliku</t>
         </is>
       </c>
-      <c r="D1" s="5" t="inlineStr">
+      <c r="D1" s="8" t="inlineStr">
         <is>
           <t>Komentarz do 1_wf</t>
         </is>
@@ -582,6 +627,91 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <cols>
+    <col width="15.81640625" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Lp</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>NR faktury</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>nazwa pliku</t>
+        </is>
+      </c>
+      <c r="D1" s="6" t="inlineStr">
+        <is>
+          <t>WF</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="inlineStr">
+        <is>
+          <t>26908/BR/2023</t>
+        </is>
+      </c>
+      <c r="C2" s="5" t="inlineStr">
+        <is>
+          <t>fv_pl_1_1bf5a3c1809c7fe44bd2e78915c3.pdf</t>
+        </is>
+      </c>
+      <c r="D2" s="5" t="inlineStr">
+        <is>
+          <t>double invoice</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="inlineStr">
+        <is>
+          <t>26908/BR/2023</t>
+        </is>
+      </c>
+      <c r="C3" s="5" t="inlineStr">
+        <is>
+          <t>fv_pl_1_1bf5a3c1809c7fe44bd2e78915c3.pdf</t>
+        </is>
+      </c>
+      <c r="D3" s="5" t="inlineStr">
+        <is>
+          <t>find second invoice</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -617,7 +747,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -668,7 +798,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -719,7 +849,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>